<commit_message>
updated K values in spreadsheet, changed bz to bx in plot_bz.py, created script to determine if magnetometers are on dayside
</commit_message>
<xml_diff>
--- a/docs/SSC_events.xlsx
+++ b/docs/SSC_events.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -67,10 +67,10 @@
     <t xml:space="preserve">50 nT</t>
   </si>
   <si>
-    <t xml:space="preserve">-1.6 x 10^-2 A/m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2 x 10^-2 A/m</t>
+    <t xml:space="preserve">2.4 x 10^-2 A/m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0 x 10^-2 A/m</t>
   </si>
   <si>
     <t xml:space="preserve">590 km/s</t>
@@ -94,7 +94,10 @@
     <t xml:space="preserve">22 nT</t>
   </si>
   <si>
-    <t xml:space="preserve">-9.5 x 10^-3 A/m</t>
+    <t xml:space="preserve">1.8 x 10^-2 A/m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.0 x 10^-2 A/m</t>
   </si>
   <si>
     <t xml:space="preserve">900 km/s</t>
@@ -109,10 +112,10 @@
     <t xml:space="preserve">15 nT</t>
   </si>
   <si>
-    <t xml:space="preserve">-8 x 10^-4 A/m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.1 x 10^-2 A/m</t>
+    <t xml:space="preserve">-4.0 x 10^-3 A/m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.0 x 10^-3 A/m</t>
   </si>
   <si>
     <t xml:space="preserve">570 km/s</t>
@@ -139,28 +142,31 @@
     <t xml:space="preserve">40 nT</t>
   </si>
   <si>
-    <t xml:space="preserve">1.3 x 10^-2 A/m</t>
+    <t xml:space="preserve">8.0 x 10^-3 A/m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4.8 x 10^-3 A/m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">720 km/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 nT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ideal event</t>
+  </si>
+  <si>
+    <t xml:space="preserve">135 nT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1 x 10^-1 A/m</t>
   </si>
   <si>
     <t xml:space="preserve">0 A/m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">720 km/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 nT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ideal event</t>
-  </si>
-  <si>
-    <t xml:space="preserve">135 nT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n/a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1 x 10^-1 A/m</t>
   </si>
   <si>
     <t xml:space="preserve">2700 km/s</t>
@@ -277,11 +283,11 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.71"/>
@@ -387,13 +393,13 @@
         <v>24</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>21</v>
@@ -402,7 +408,7 @@
         <v>20</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,28 +425,28 @@
         <v>20</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -451,60 +457,60 @@
         <v>0.24375</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>20</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>